<commit_message>
EPBDS-11198 behaviour for 'java.lang.Void' must be the same as for 'void' primitive
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11198_Decision_Void_retType.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11198_Decision_Void_retType.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpikus\.openl-webstudio\user-workspace\DEFAULT\Sample Project111\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\demo,war\5.24.1_17.03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570C1496-B431-42BE-BFAC-54D9D0D2171B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F547DADD-3B5C-4E02-8F9A-B253B1EC4EE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1695" windowWidth="25980" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="42">
   <si>
     <t>= null</t>
   </si>
@@ -47,16 +58,121 @@
   </si>
   <si>
     <t>_res_</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Young Driver</t>
+  </si>
+  <si>
+    <t>Senior Driver</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>driverAge</t>
+  </si>
+  <si>
+    <t>driverMaritalStatus</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Driver Age</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Premium Increase</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Test doVoidSimpleL</t>
+  </si>
+  <si>
+    <t>SimpleRules void doVoidSimple (String driverAge, String driverMaritalStatus)</t>
+  </si>
+  <si>
+    <t>Test doVoidSimple</t>
+  </si>
+  <si>
+    <t>Rules void doVoidRules (String driverAge, String driverMaritalStatus)</t>
+  </si>
+  <si>
+    <t>Test doVoidRules</t>
+  </si>
+  <si>
+    <t>Test doVoidSmartL</t>
+  </si>
+  <si>
+    <t>Age
+                Marital Status</t>
+  </si>
+  <si>
+    <t>=null</t>
+  </si>
+  <si>
+    <t>SmartLookup void doVoidSmartL(String Age, String Status)</t>
+  </si>
+  <si>
+    <t>=700</t>
+  </si>
+  <si>
+    <t>=300</t>
+  </si>
+  <si>
+    <t>=720</t>
+  </si>
+  <si>
+    <t>=350</t>
+  </si>
+  <si>
+    <t>=78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age </t>
+  </si>
+  <si>
+    <t>SmartRules Void doVoidSmart2(String foo)</t>
+  </si>
+  <si>
+    <t>Test doVoidSmart2</t>
+  </si>
+  <si>
+    <t>SimpleLookup Void doVoidSimpleL(String Age, String Status)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -79,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -87,9 +203,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -452,80 +604,550 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:C18"/>
+  <dimension ref="B6:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="18" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" style="1" collapsed="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="13" width="9.140625" style="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="G6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="L6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+    </row>
+    <row r="7" spans="2:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="G7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="G16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="9"/>
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="6"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" s="9"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="9"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="12"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G37" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G38" s="9"/>
+      <c r="H38" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="11"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B44" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="11"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B52" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="11"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B53" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="O24:Q24"/>
+  </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>